<commit_message>
Modified a gamepad diagram
</commit_message>
<xml_diff>
--- a/HTML5-XInput-locations.xlsx
+++ b/HTML5-XInput-locations.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TAKIZAWA Yozo\github\ytaki0801.github.io\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TAKIZAWA Yozo\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{019B901D-B231-4D2B-96D6-B2536DDB69A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F04D6430-5C8C-412F-9FFB-B9123DCCCE4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{38F73DDA-D621-463A-9F7D-10B89270610F}"/>
   </bookViews>
@@ -79,99 +79,12 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="1">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -180,7 +93,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -190,28 +103,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -370,16 +262,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>228600</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -390,12 +282,15 @@
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="6" idx="0"/>
+          <a:endCxn id="13" idx="0"/>
+        </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="1905000" y="1895475"/>
-          <a:ext cx="4057650" cy="9525"/>
+          <a:off x="2400300" y="1905000"/>
+          <a:ext cx="3067050" cy="9525"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -426,15 +321,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>228600</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -445,12 +340,15 @@
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="6" idx="2"/>
+          <a:endCxn id="4" idx="2"/>
+        </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="1438275" y="1905000"/>
-          <a:ext cx="457200" cy="2867025"/>
+          <a:off x="1428750" y="2619375"/>
+          <a:ext cx="381000" cy="1895475"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -483,13 +381,13 @@
       <xdr:col>10</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -504,7 +402,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2381250" y="4067175"/>
+          <a:off x="2381250" y="4057650"/>
           <a:ext cx="3105150" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -535,125 +433,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>228600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
+      <xdr:col>27</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="10" name="直線コネクタ 9">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E387BC55-C9F4-4222-80C3-BCF73AADC323}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="2133600" y="4057650"/>
-          <a:ext cx="247650" cy="714375"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:solidFill>
-            <a:sysClr val="windowText" lastClr="000000"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="12" name="直線コネクタ 11">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2ACE202F-A013-48BB-A94E-42394B5CFE9E}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1438275" y="4762500"/>
-          <a:ext cx="676275" cy="9525"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:solidFill>
-            <a:sysClr val="windowText" lastClr="000000"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>219075</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>219075</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -669,8 +457,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5953125" y="1885950"/>
-          <a:ext cx="457200" cy="2886075"/>
+          <a:off x="6076950" y="2609850"/>
+          <a:ext cx="352425" cy="1924050"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -700,36 +488,123 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="19" name="直線コネクタ 18">
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="フリーフォーム: 図形 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{78B87727-6D84-4C36-9380-442DD091928E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6A33550D-8B96-F753-2BED-8F261D427AE9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5476875" y="4067175"/>
-          <a:ext cx="238125" cy="704850"/>
+          <a:off x="1809750" y="1914525"/>
+          <a:ext cx="590550" cy="704850"/>
         </a:xfrm>
-        <a:prstGeom prst="line">
+        <a:custGeom>
           <a:avLst/>
-        </a:prstGeom>
+          <a:gdLst>
+            <a:gd name="connsiteX0" fmla="*/ 714375 w 714375"/>
+            <a:gd name="connsiteY0" fmla="*/ 0 h 704850"/>
+            <a:gd name="connsiteX1" fmla="*/ 238125 w 714375"/>
+            <a:gd name="connsiteY1" fmla="*/ 228600 h 704850"/>
+            <a:gd name="connsiteX2" fmla="*/ 0 w 714375"/>
+            <a:gd name="connsiteY2" fmla="*/ 704850 h 704850"/>
+            <a:gd name="connsiteX0" fmla="*/ 714375 w 714375"/>
+            <a:gd name="connsiteY0" fmla="*/ 0 h 704850"/>
+            <a:gd name="connsiteX1" fmla="*/ 114300 w 714375"/>
+            <a:gd name="connsiteY1" fmla="*/ 114300 h 704850"/>
+            <a:gd name="connsiteX2" fmla="*/ 0 w 714375"/>
+            <a:gd name="connsiteY2" fmla="*/ 704850 h 704850"/>
+            <a:gd name="connsiteX0" fmla="*/ 714375 w 714375"/>
+            <a:gd name="connsiteY0" fmla="*/ 0 h 704850"/>
+            <a:gd name="connsiteX1" fmla="*/ 171450 w 714375"/>
+            <a:gd name="connsiteY1" fmla="*/ 152400 h 704850"/>
+            <a:gd name="connsiteX2" fmla="*/ 0 w 714375"/>
+            <a:gd name="connsiteY2" fmla="*/ 704850 h 704850"/>
+            <a:gd name="connsiteX0" fmla="*/ 714375 w 714375"/>
+            <a:gd name="connsiteY0" fmla="*/ 0 h 704850"/>
+            <a:gd name="connsiteX1" fmla="*/ 238125 w 714375"/>
+            <a:gd name="connsiteY1" fmla="*/ 219075 h 704850"/>
+            <a:gd name="connsiteX2" fmla="*/ 0 w 714375"/>
+            <a:gd name="connsiteY2" fmla="*/ 704850 h 704850"/>
+            <a:gd name="connsiteX0" fmla="*/ 581025 w 581025"/>
+            <a:gd name="connsiteY0" fmla="*/ 0 h 704850"/>
+            <a:gd name="connsiteX1" fmla="*/ 104775 w 581025"/>
+            <a:gd name="connsiteY1" fmla="*/ 219075 h 704850"/>
+            <a:gd name="connsiteX2" fmla="*/ 0 w 581025"/>
+            <a:gd name="connsiteY2" fmla="*/ 704850 h 704850"/>
+            <a:gd name="connsiteX0" fmla="*/ 609600 w 609600"/>
+            <a:gd name="connsiteY0" fmla="*/ 0 h 704850"/>
+            <a:gd name="connsiteX1" fmla="*/ 133350 w 609600"/>
+            <a:gd name="connsiteY1" fmla="*/ 219075 h 704850"/>
+            <a:gd name="connsiteX2" fmla="*/ 0 w 609600"/>
+            <a:gd name="connsiteY2" fmla="*/ 704850 h 704850"/>
+            <a:gd name="connsiteX0" fmla="*/ 609600 w 609600"/>
+            <a:gd name="connsiteY0" fmla="*/ 0 h 704850"/>
+            <a:gd name="connsiteX1" fmla="*/ 238125 w 609600"/>
+            <a:gd name="connsiteY1" fmla="*/ 123825 h 704850"/>
+            <a:gd name="connsiteX2" fmla="*/ 0 w 609600"/>
+            <a:gd name="connsiteY2" fmla="*/ 704850 h 704850"/>
+            <a:gd name="connsiteX0" fmla="*/ 609600 w 609600"/>
+            <a:gd name="connsiteY0" fmla="*/ 0 h 704850"/>
+            <a:gd name="connsiteX1" fmla="*/ 295275 w 609600"/>
+            <a:gd name="connsiteY1" fmla="*/ 171450 h 704850"/>
+            <a:gd name="connsiteX2" fmla="*/ 0 w 609600"/>
+            <a:gd name="connsiteY2" fmla="*/ 704850 h 704850"/>
+            <a:gd name="connsiteX0" fmla="*/ 590550 w 590550"/>
+            <a:gd name="connsiteY0" fmla="*/ 0 h 704850"/>
+            <a:gd name="connsiteX1" fmla="*/ 276225 w 590550"/>
+            <a:gd name="connsiteY1" fmla="*/ 171450 h 704850"/>
+            <a:gd name="connsiteX2" fmla="*/ 0 w 590550"/>
+            <a:gd name="connsiteY2" fmla="*/ 704850 h 704850"/>
+          </a:gdLst>
+          <a:ahLst/>
+          <a:cxnLst>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX0" y="connsiteY0"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX1" y="connsiteY1"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX2" y="connsiteY2"/>
+            </a:cxn>
+          </a:cxnLst>
+          <a:rect l="l" t="t" r="r" b="b"/>
+          <a:pathLst>
+            <a:path w="590550" h="704850">
+              <a:moveTo>
+                <a:pt x="590550" y="0"/>
+              </a:moveTo>
+              <a:cubicBezTo>
+                <a:pt x="411956" y="55562"/>
+                <a:pt x="374650" y="53975"/>
+                <a:pt x="276225" y="171450"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="177800" y="288925"/>
+                <a:pt x="59531" y="525462"/>
+                <a:pt x="0" y="704850"/>
+              </a:cubicBezTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
         <a:ln>
           <a:solidFill>
             <a:sysClr val="windowText" lastClr="000000"/>
@@ -737,54 +612,151 @@
         </a:ln>
       </xdr:spPr>
       <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
         </a:lnRef>
-        <a:fillRef idx="0">
+        <a:fillRef idx="1">
           <a:schemeClr val="accent1"/>
         </a:fillRef>
         <a:effectRef idx="0">
           <a:schemeClr val="accent1"/>
         </a:effectRef>
         <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
+          <a:schemeClr val="lt1"/>
         </a:fontRef>
       </xdr:style>
-    </xdr:cxnSp>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>228600</xdr:rowOff>
     </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="21" name="直線コネクタ 20">
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="フリーフォーム: 図形 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{61B1D3D4-833B-4B58-8307-81426161E168}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5BA16D33-9986-4F3A-A351-242575EDAAB4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5715000" y="4762500"/>
-          <a:ext cx="676275" cy="9525"/>
+        <a:xfrm flipH="1">
+          <a:off x="5467350" y="1905000"/>
+          <a:ext cx="609600" cy="704850"/>
         </a:xfrm>
-        <a:prstGeom prst="line">
+        <a:custGeom>
           <a:avLst/>
-        </a:prstGeom>
+          <a:gdLst>
+            <a:gd name="connsiteX0" fmla="*/ 714375 w 714375"/>
+            <a:gd name="connsiteY0" fmla="*/ 0 h 704850"/>
+            <a:gd name="connsiteX1" fmla="*/ 238125 w 714375"/>
+            <a:gd name="connsiteY1" fmla="*/ 228600 h 704850"/>
+            <a:gd name="connsiteX2" fmla="*/ 0 w 714375"/>
+            <a:gd name="connsiteY2" fmla="*/ 704850 h 704850"/>
+            <a:gd name="connsiteX0" fmla="*/ 714375 w 714375"/>
+            <a:gd name="connsiteY0" fmla="*/ 0 h 704850"/>
+            <a:gd name="connsiteX1" fmla="*/ 114300 w 714375"/>
+            <a:gd name="connsiteY1" fmla="*/ 114300 h 704850"/>
+            <a:gd name="connsiteX2" fmla="*/ 0 w 714375"/>
+            <a:gd name="connsiteY2" fmla="*/ 704850 h 704850"/>
+            <a:gd name="connsiteX0" fmla="*/ 714375 w 714375"/>
+            <a:gd name="connsiteY0" fmla="*/ 0 h 704850"/>
+            <a:gd name="connsiteX1" fmla="*/ 171450 w 714375"/>
+            <a:gd name="connsiteY1" fmla="*/ 152400 h 704850"/>
+            <a:gd name="connsiteX2" fmla="*/ 0 w 714375"/>
+            <a:gd name="connsiteY2" fmla="*/ 704850 h 704850"/>
+            <a:gd name="connsiteX0" fmla="*/ 714375 w 714375"/>
+            <a:gd name="connsiteY0" fmla="*/ 0 h 704850"/>
+            <a:gd name="connsiteX1" fmla="*/ 238125 w 714375"/>
+            <a:gd name="connsiteY1" fmla="*/ 219075 h 704850"/>
+            <a:gd name="connsiteX2" fmla="*/ 0 w 714375"/>
+            <a:gd name="connsiteY2" fmla="*/ 704850 h 704850"/>
+            <a:gd name="connsiteX0" fmla="*/ 581025 w 581025"/>
+            <a:gd name="connsiteY0" fmla="*/ 0 h 704850"/>
+            <a:gd name="connsiteX1" fmla="*/ 104775 w 581025"/>
+            <a:gd name="connsiteY1" fmla="*/ 219075 h 704850"/>
+            <a:gd name="connsiteX2" fmla="*/ 0 w 581025"/>
+            <a:gd name="connsiteY2" fmla="*/ 704850 h 704850"/>
+            <a:gd name="connsiteX0" fmla="*/ 609600 w 609600"/>
+            <a:gd name="connsiteY0" fmla="*/ 0 h 704850"/>
+            <a:gd name="connsiteX1" fmla="*/ 133350 w 609600"/>
+            <a:gd name="connsiteY1" fmla="*/ 219075 h 704850"/>
+            <a:gd name="connsiteX2" fmla="*/ 0 w 609600"/>
+            <a:gd name="connsiteY2" fmla="*/ 704850 h 704850"/>
+            <a:gd name="connsiteX0" fmla="*/ 609600 w 609600"/>
+            <a:gd name="connsiteY0" fmla="*/ 0 h 704850"/>
+            <a:gd name="connsiteX1" fmla="*/ 238125 w 609600"/>
+            <a:gd name="connsiteY1" fmla="*/ 123825 h 704850"/>
+            <a:gd name="connsiteX2" fmla="*/ 0 w 609600"/>
+            <a:gd name="connsiteY2" fmla="*/ 704850 h 704850"/>
+            <a:gd name="connsiteX0" fmla="*/ 609600 w 609600"/>
+            <a:gd name="connsiteY0" fmla="*/ 0 h 704850"/>
+            <a:gd name="connsiteX1" fmla="*/ 295275 w 609600"/>
+            <a:gd name="connsiteY1" fmla="*/ 171450 h 704850"/>
+            <a:gd name="connsiteX2" fmla="*/ 0 w 609600"/>
+            <a:gd name="connsiteY2" fmla="*/ 704850 h 704850"/>
+            <a:gd name="connsiteX0" fmla="*/ 590550 w 590550"/>
+            <a:gd name="connsiteY0" fmla="*/ 0 h 704850"/>
+            <a:gd name="connsiteX1" fmla="*/ 276225 w 590550"/>
+            <a:gd name="connsiteY1" fmla="*/ 171450 h 704850"/>
+            <a:gd name="connsiteX2" fmla="*/ 0 w 590550"/>
+            <a:gd name="connsiteY2" fmla="*/ 704850 h 704850"/>
+          </a:gdLst>
+          <a:ahLst/>
+          <a:cxnLst>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX0" y="connsiteY0"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX1" y="connsiteY1"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX2" y="connsiteY2"/>
+            </a:cxn>
+          </a:cxnLst>
+          <a:rect l="l" t="t" r="r" b="b"/>
+          <a:pathLst>
+            <a:path w="590550" h="704850">
+              <a:moveTo>
+                <a:pt x="590550" y="0"/>
+              </a:moveTo>
+              <a:cubicBezTo>
+                <a:pt x="411956" y="55562"/>
+                <a:pt x="374650" y="53975"/>
+                <a:pt x="276225" y="171450"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="177800" y="288925"/>
+                <a:pt x="59531" y="525462"/>
+                <a:pt x="0" y="704850"/>
+              </a:cubicBezTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
         <a:ln>
           <a:solidFill>
             <a:sysClr val="windowText" lastClr="000000"/>
@@ -792,20 +764,1612 @@
         </a:ln>
       </xdr:spPr>
       <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
         </a:lnRef>
-        <a:fillRef idx="0">
+        <a:fillRef idx="1">
           <a:schemeClr val="accent1"/>
         </a:fillRef>
         <a:effectRef idx="0">
           <a:schemeClr val="accent1"/>
         </a:effectRef>
         <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
+          <a:schemeClr val="lt1"/>
         </a:fontRef>
       </xdr:style>
-    </xdr:cxnSp>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="四角形: 角を丸くする 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B09D16DA-23F4-AAF4-1A05-8D52B37DAC23}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2628900" y="723900"/>
+          <a:ext cx="219075" cy="466725"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>228600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="フリーフォーム: 図形 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A7145DF-57EB-4671-983F-7E1B8CF82DDA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1428750" y="4514850"/>
+          <a:ext cx="466725" cy="257174"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst>
+            <a:gd name="connsiteX0" fmla="*/ 714375 w 714375"/>
+            <a:gd name="connsiteY0" fmla="*/ 0 h 704850"/>
+            <a:gd name="connsiteX1" fmla="*/ 238125 w 714375"/>
+            <a:gd name="connsiteY1" fmla="*/ 228600 h 704850"/>
+            <a:gd name="connsiteX2" fmla="*/ 0 w 714375"/>
+            <a:gd name="connsiteY2" fmla="*/ 704850 h 704850"/>
+            <a:gd name="connsiteX0" fmla="*/ 714375 w 714375"/>
+            <a:gd name="connsiteY0" fmla="*/ 0 h 704850"/>
+            <a:gd name="connsiteX1" fmla="*/ 114300 w 714375"/>
+            <a:gd name="connsiteY1" fmla="*/ 114300 h 704850"/>
+            <a:gd name="connsiteX2" fmla="*/ 0 w 714375"/>
+            <a:gd name="connsiteY2" fmla="*/ 704850 h 704850"/>
+            <a:gd name="connsiteX0" fmla="*/ 714375 w 714375"/>
+            <a:gd name="connsiteY0" fmla="*/ 0 h 704850"/>
+            <a:gd name="connsiteX1" fmla="*/ 171450 w 714375"/>
+            <a:gd name="connsiteY1" fmla="*/ 152400 h 704850"/>
+            <a:gd name="connsiteX2" fmla="*/ 0 w 714375"/>
+            <a:gd name="connsiteY2" fmla="*/ 704850 h 704850"/>
+            <a:gd name="connsiteX0" fmla="*/ 714375 w 714375"/>
+            <a:gd name="connsiteY0" fmla="*/ 0 h 704850"/>
+            <a:gd name="connsiteX1" fmla="*/ 238125 w 714375"/>
+            <a:gd name="connsiteY1" fmla="*/ 219075 h 704850"/>
+            <a:gd name="connsiteX2" fmla="*/ 0 w 714375"/>
+            <a:gd name="connsiteY2" fmla="*/ 704850 h 704850"/>
+            <a:gd name="connsiteX0" fmla="*/ 581025 w 581025"/>
+            <a:gd name="connsiteY0" fmla="*/ 0 h 704850"/>
+            <a:gd name="connsiteX1" fmla="*/ 104775 w 581025"/>
+            <a:gd name="connsiteY1" fmla="*/ 219075 h 704850"/>
+            <a:gd name="connsiteX2" fmla="*/ 0 w 581025"/>
+            <a:gd name="connsiteY2" fmla="*/ 704850 h 704850"/>
+            <a:gd name="connsiteX0" fmla="*/ 609600 w 609600"/>
+            <a:gd name="connsiteY0" fmla="*/ 0 h 704850"/>
+            <a:gd name="connsiteX1" fmla="*/ 133350 w 609600"/>
+            <a:gd name="connsiteY1" fmla="*/ 219075 h 704850"/>
+            <a:gd name="connsiteX2" fmla="*/ 0 w 609600"/>
+            <a:gd name="connsiteY2" fmla="*/ 704850 h 704850"/>
+            <a:gd name="connsiteX0" fmla="*/ 609600 w 609600"/>
+            <a:gd name="connsiteY0" fmla="*/ 0 h 704850"/>
+            <a:gd name="connsiteX1" fmla="*/ 238125 w 609600"/>
+            <a:gd name="connsiteY1" fmla="*/ 123825 h 704850"/>
+            <a:gd name="connsiteX2" fmla="*/ 0 w 609600"/>
+            <a:gd name="connsiteY2" fmla="*/ 704850 h 704850"/>
+            <a:gd name="connsiteX0" fmla="*/ 609600 w 609600"/>
+            <a:gd name="connsiteY0" fmla="*/ 0 h 704850"/>
+            <a:gd name="connsiteX1" fmla="*/ 295275 w 609600"/>
+            <a:gd name="connsiteY1" fmla="*/ 171450 h 704850"/>
+            <a:gd name="connsiteX2" fmla="*/ 0 w 609600"/>
+            <a:gd name="connsiteY2" fmla="*/ 704850 h 704850"/>
+            <a:gd name="connsiteX0" fmla="*/ 590550 w 590550"/>
+            <a:gd name="connsiteY0" fmla="*/ 0 h 704850"/>
+            <a:gd name="connsiteX1" fmla="*/ 276225 w 590550"/>
+            <a:gd name="connsiteY1" fmla="*/ 171450 h 704850"/>
+            <a:gd name="connsiteX2" fmla="*/ 0 w 590550"/>
+            <a:gd name="connsiteY2" fmla="*/ 704850 h 704850"/>
+          </a:gdLst>
+          <a:ahLst/>
+          <a:cxnLst>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX0" y="connsiteY0"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX1" y="connsiteY1"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX2" y="connsiteY2"/>
+            </a:cxn>
+          </a:cxnLst>
+          <a:rect l="l" t="t" r="r" b="b"/>
+          <a:pathLst>
+            <a:path w="590550" h="704850">
+              <a:moveTo>
+                <a:pt x="590550" y="0"/>
+              </a:moveTo>
+              <a:cubicBezTo>
+                <a:pt x="411956" y="55562"/>
+                <a:pt x="374650" y="53975"/>
+                <a:pt x="276225" y="171450"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="177800" y="288925"/>
+                <a:pt x="59531" y="525462"/>
+                <a:pt x="0" y="704850"/>
+              </a:cubicBezTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>228600</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="四角形: 角を丸くする 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BC372D7D-F8FD-437C-8A6A-9A694A25EFA5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5000625" y="714375"/>
+          <a:ext cx="219075" cy="466725"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>219073</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>9523</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="フリーフォーム: 図形 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EB863652-1B3F-4646-99A5-AE9BFD75C5A0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="1885948" y="4057650"/>
+          <a:ext cx="504825" cy="714374"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst>
+            <a:gd name="connsiteX0" fmla="*/ 714375 w 714375"/>
+            <a:gd name="connsiteY0" fmla="*/ 0 h 704850"/>
+            <a:gd name="connsiteX1" fmla="*/ 238125 w 714375"/>
+            <a:gd name="connsiteY1" fmla="*/ 228600 h 704850"/>
+            <a:gd name="connsiteX2" fmla="*/ 0 w 714375"/>
+            <a:gd name="connsiteY2" fmla="*/ 704850 h 704850"/>
+            <a:gd name="connsiteX0" fmla="*/ 714375 w 714375"/>
+            <a:gd name="connsiteY0" fmla="*/ 0 h 704850"/>
+            <a:gd name="connsiteX1" fmla="*/ 114300 w 714375"/>
+            <a:gd name="connsiteY1" fmla="*/ 114300 h 704850"/>
+            <a:gd name="connsiteX2" fmla="*/ 0 w 714375"/>
+            <a:gd name="connsiteY2" fmla="*/ 704850 h 704850"/>
+            <a:gd name="connsiteX0" fmla="*/ 714375 w 714375"/>
+            <a:gd name="connsiteY0" fmla="*/ 0 h 704850"/>
+            <a:gd name="connsiteX1" fmla="*/ 171450 w 714375"/>
+            <a:gd name="connsiteY1" fmla="*/ 152400 h 704850"/>
+            <a:gd name="connsiteX2" fmla="*/ 0 w 714375"/>
+            <a:gd name="connsiteY2" fmla="*/ 704850 h 704850"/>
+            <a:gd name="connsiteX0" fmla="*/ 714375 w 714375"/>
+            <a:gd name="connsiteY0" fmla="*/ 0 h 704850"/>
+            <a:gd name="connsiteX1" fmla="*/ 238125 w 714375"/>
+            <a:gd name="connsiteY1" fmla="*/ 219075 h 704850"/>
+            <a:gd name="connsiteX2" fmla="*/ 0 w 714375"/>
+            <a:gd name="connsiteY2" fmla="*/ 704850 h 704850"/>
+            <a:gd name="connsiteX0" fmla="*/ 581025 w 581025"/>
+            <a:gd name="connsiteY0" fmla="*/ 0 h 704850"/>
+            <a:gd name="connsiteX1" fmla="*/ 104775 w 581025"/>
+            <a:gd name="connsiteY1" fmla="*/ 219075 h 704850"/>
+            <a:gd name="connsiteX2" fmla="*/ 0 w 581025"/>
+            <a:gd name="connsiteY2" fmla="*/ 704850 h 704850"/>
+            <a:gd name="connsiteX0" fmla="*/ 609600 w 609600"/>
+            <a:gd name="connsiteY0" fmla="*/ 0 h 704850"/>
+            <a:gd name="connsiteX1" fmla="*/ 133350 w 609600"/>
+            <a:gd name="connsiteY1" fmla="*/ 219075 h 704850"/>
+            <a:gd name="connsiteX2" fmla="*/ 0 w 609600"/>
+            <a:gd name="connsiteY2" fmla="*/ 704850 h 704850"/>
+            <a:gd name="connsiteX0" fmla="*/ 609600 w 609600"/>
+            <a:gd name="connsiteY0" fmla="*/ 0 h 704850"/>
+            <a:gd name="connsiteX1" fmla="*/ 238125 w 609600"/>
+            <a:gd name="connsiteY1" fmla="*/ 123825 h 704850"/>
+            <a:gd name="connsiteX2" fmla="*/ 0 w 609600"/>
+            <a:gd name="connsiteY2" fmla="*/ 704850 h 704850"/>
+            <a:gd name="connsiteX0" fmla="*/ 609600 w 609600"/>
+            <a:gd name="connsiteY0" fmla="*/ 0 h 704850"/>
+            <a:gd name="connsiteX1" fmla="*/ 295275 w 609600"/>
+            <a:gd name="connsiteY1" fmla="*/ 171450 h 704850"/>
+            <a:gd name="connsiteX2" fmla="*/ 0 w 609600"/>
+            <a:gd name="connsiteY2" fmla="*/ 704850 h 704850"/>
+            <a:gd name="connsiteX0" fmla="*/ 590550 w 590550"/>
+            <a:gd name="connsiteY0" fmla="*/ 0 h 704850"/>
+            <a:gd name="connsiteX1" fmla="*/ 276225 w 590550"/>
+            <a:gd name="connsiteY1" fmla="*/ 171450 h 704850"/>
+            <a:gd name="connsiteX2" fmla="*/ 0 w 590550"/>
+            <a:gd name="connsiteY2" fmla="*/ 704850 h 704850"/>
+          </a:gdLst>
+          <a:ahLst/>
+          <a:cxnLst>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX0" y="connsiteY0"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX1" y="connsiteY1"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX2" y="connsiteY2"/>
+            </a:cxn>
+          </a:cxnLst>
+          <a:rect l="l" t="t" r="r" b="b"/>
+          <a:pathLst>
+            <a:path w="590550" h="704850">
+              <a:moveTo>
+                <a:pt x="590550" y="0"/>
+              </a:moveTo>
+              <a:cubicBezTo>
+                <a:pt x="411956" y="55562"/>
+                <a:pt x="374650" y="53975"/>
+                <a:pt x="276225" y="171450"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="177800" y="288925"/>
+                <a:pt x="59531" y="525462"/>
+                <a:pt x="0" y="704850"/>
+              </a:cubicBezTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>9522</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>9524</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="25" name="フリーフォーム: 図形 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A98216A-902A-485C-8E29-E5EB45132EAD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="5486397" y="4057650"/>
+          <a:ext cx="476252" cy="714374"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst>
+            <a:gd name="connsiteX0" fmla="*/ 714375 w 714375"/>
+            <a:gd name="connsiteY0" fmla="*/ 0 h 704850"/>
+            <a:gd name="connsiteX1" fmla="*/ 238125 w 714375"/>
+            <a:gd name="connsiteY1" fmla="*/ 228600 h 704850"/>
+            <a:gd name="connsiteX2" fmla="*/ 0 w 714375"/>
+            <a:gd name="connsiteY2" fmla="*/ 704850 h 704850"/>
+            <a:gd name="connsiteX0" fmla="*/ 714375 w 714375"/>
+            <a:gd name="connsiteY0" fmla="*/ 0 h 704850"/>
+            <a:gd name="connsiteX1" fmla="*/ 114300 w 714375"/>
+            <a:gd name="connsiteY1" fmla="*/ 114300 h 704850"/>
+            <a:gd name="connsiteX2" fmla="*/ 0 w 714375"/>
+            <a:gd name="connsiteY2" fmla="*/ 704850 h 704850"/>
+            <a:gd name="connsiteX0" fmla="*/ 714375 w 714375"/>
+            <a:gd name="connsiteY0" fmla="*/ 0 h 704850"/>
+            <a:gd name="connsiteX1" fmla="*/ 171450 w 714375"/>
+            <a:gd name="connsiteY1" fmla="*/ 152400 h 704850"/>
+            <a:gd name="connsiteX2" fmla="*/ 0 w 714375"/>
+            <a:gd name="connsiteY2" fmla="*/ 704850 h 704850"/>
+            <a:gd name="connsiteX0" fmla="*/ 714375 w 714375"/>
+            <a:gd name="connsiteY0" fmla="*/ 0 h 704850"/>
+            <a:gd name="connsiteX1" fmla="*/ 238125 w 714375"/>
+            <a:gd name="connsiteY1" fmla="*/ 219075 h 704850"/>
+            <a:gd name="connsiteX2" fmla="*/ 0 w 714375"/>
+            <a:gd name="connsiteY2" fmla="*/ 704850 h 704850"/>
+            <a:gd name="connsiteX0" fmla="*/ 581025 w 581025"/>
+            <a:gd name="connsiteY0" fmla="*/ 0 h 704850"/>
+            <a:gd name="connsiteX1" fmla="*/ 104775 w 581025"/>
+            <a:gd name="connsiteY1" fmla="*/ 219075 h 704850"/>
+            <a:gd name="connsiteX2" fmla="*/ 0 w 581025"/>
+            <a:gd name="connsiteY2" fmla="*/ 704850 h 704850"/>
+            <a:gd name="connsiteX0" fmla="*/ 609600 w 609600"/>
+            <a:gd name="connsiteY0" fmla="*/ 0 h 704850"/>
+            <a:gd name="connsiteX1" fmla="*/ 133350 w 609600"/>
+            <a:gd name="connsiteY1" fmla="*/ 219075 h 704850"/>
+            <a:gd name="connsiteX2" fmla="*/ 0 w 609600"/>
+            <a:gd name="connsiteY2" fmla="*/ 704850 h 704850"/>
+            <a:gd name="connsiteX0" fmla="*/ 609600 w 609600"/>
+            <a:gd name="connsiteY0" fmla="*/ 0 h 704850"/>
+            <a:gd name="connsiteX1" fmla="*/ 238125 w 609600"/>
+            <a:gd name="connsiteY1" fmla="*/ 123825 h 704850"/>
+            <a:gd name="connsiteX2" fmla="*/ 0 w 609600"/>
+            <a:gd name="connsiteY2" fmla="*/ 704850 h 704850"/>
+            <a:gd name="connsiteX0" fmla="*/ 609600 w 609600"/>
+            <a:gd name="connsiteY0" fmla="*/ 0 h 704850"/>
+            <a:gd name="connsiteX1" fmla="*/ 295275 w 609600"/>
+            <a:gd name="connsiteY1" fmla="*/ 171450 h 704850"/>
+            <a:gd name="connsiteX2" fmla="*/ 0 w 609600"/>
+            <a:gd name="connsiteY2" fmla="*/ 704850 h 704850"/>
+            <a:gd name="connsiteX0" fmla="*/ 590550 w 590550"/>
+            <a:gd name="connsiteY0" fmla="*/ 0 h 704850"/>
+            <a:gd name="connsiteX1" fmla="*/ 276225 w 590550"/>
+            <a:gd name="connsiteY1" fmla="*/ 171450 h 704850"/>
+            <a:gd name="connsiteX2" fmla="*/ 0 w 590550"/>
+            <a:gd name="connsiteY2" fmla="*/ 704850 h 704850"/>
+          </a:gdLst>
+          <a:ahLst/>
+          <a:cxnLst>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX0" y="connsiteY0"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX1" y="connsiteY1"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX2" y="connsiteY2"/>
+            </a:cxn>
+          </a:cxnLst>
+          <a:rect l="l" t="t" r="r" b="b"/>
+          <a:pathLst>
+            <a:path w="590550" h="704850">
+              <a:moveTo>
+                <a:pt x="590550" y="0"/>
+              </a:moveTo>
+              <a:cubicBezTo>
+                <a:pt x="411956" y="55562"/>
+                <a:pt x="374650" y="53975"/>
+                <a:pt x="276225" y="171450"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="177800" y="288925"/>
+                <a:pt x="59531" y="525462"/>
+                <a:pt x="0" y="704850"/>
+              </a:cubicBezTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>238124</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>238124</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="38" name="フリーフォーム: 図形 37">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CD7136F8-E868-4519-A022-EAF19A6F380B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="5943600" y="4524374"/>
+          <a:ext cx="485776" cy="238125"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst>
+            <a:gd name="connsiteX0" fmla="*/ 714375 w 714375"/>
+            <a:gd name="connsiteY0" fmla="*/ 0 h 704850"/>
+            <a:gd name="connsiteX1" fmla="*/ 238125 w 714375"/>
+            <a:gd name="connsiteY1" fmla="*/ 228600 h 704850"/>
+            <a:gd name="connsiteX2" fmla="*/ 0 w 714375"/>
+            <a:gd name="connsiteY2" fmla="*/ 704850 h 704850"/>
+            <a:gd name="connsiteX0" fmla="*/ 714375 w 714375"/>
+            <a:gd name="connsiteY0" fmla="*/ 0 h 704850"/>
+            <a:gd name="connsiteX1" fmla="*/ 114300 w 714375"/>
+            <a:gd name="connsiteY1" fmla="*/ 114300 h 704850"/>
+            <a:gd name="connsiteX2" fmla="*/ 0 w 714375"/>
+            <a:gd name="connsiteY2" fmla="*/ 704850 h 704850"/>
+            <a:gd name="connsiteX0" fmla="*/ 714375 w 714375"/>
+            <a:gd name="connsiteY0" fmla="*/ 0 h 704850"/>
+            <a:gd name="connsiteX1" fmla="*/ 171450 w 714375"/>
+            <a:gd name="connsiteY1" fmla="*/ 152400 h 704850"/>
+            <a:gd name="connsiteX2" fmla="*/ 0 w 714375"/>
+            <a:gd name="connsiteY2" fmla="*/ 704850 h 704850"/>
+            <a:gd name="connsiteX0" fmla="*/ 714375 w 714375"/>
+            <a:gd name="connsiteY0" fmla="*/ 0 h 704850"/>
+            <a:gd name="connsiteX1" fmla="*/ 238125 w 714375"/>
+            <a:gd name="connsiteY1" fmla="*/ 219075 h 704850"/>
+            <a:gd name="connsiteX2" fmla="*/ 0 w 714375"/>
+            <a:gd name="connsiteY2" fmla="*/ 704850 h 704850"/>
+            <a:gd name="connsiteX0" fmla="*/ 581025 w 581025"/>
+            <a:gd name="connsiteY0" fmla="*/ 0 h 704850"/>
+            <a:gd name="connsiteX1" fmla="*/ 104775 w 581025"/>
+            <a:gd name="connsiteY1" fmla="*/ 219075 h 704850"/>
+            <a:gd name="connsiteX2" fmla="*/ 0 w 581025"/>
+            <a:gd name="connsiteY2" fmla="*/ 704850 h 704850"/>
+            <a:gd name="connsiteX0" fmla="*/ 609600 w 609600"/>
+            <a:gd name="connsiteY0" fmla="*/ 0 h 704850"/>
+            <a:gd name="connsiteX1" fmla="*/ 133350 w 609600"/>
+            <a:gd name="connsiteY1" fmla="*/ 219075 h 704850"/>
+            <a:gd name="connsiteX2" fmla="*/ 0 w 609600"/>
+            <a:gd name="connsiteY2" fmla="*/ 704850 h 704850"/>
+            <a:gd name="connsiteX0" fmla="*/ 609600 w 609600"/>
+            <a:gd name="connsiteY0" fmla="*/ 0 h 704850"/>
+            <a:gd name="connsiteX1" fmla="*/ 238125 w 609600"/>
+            <a:gd name="connsiteY1" fmla="*/ 123825 h 704850"/>
+            <a:gd name="connsiteX2" fmla="*/ 0 w 609600"/>
+            <a:gd name="connsiteY2" fmla="*/ 704850 h 704850"/>
+            <a:gd name="connsiteX0" fmla="*/ 609600 w 609600"/>
+            <a:gd name="connsiteY0" fmla="*/ 0 h 704850"/>
+            <a:gd name="connsiteX1" fmla="*/ 295275 w 609600"/>
+            <a:gd name="connsiteY1" fmla="*/ 171450 h 704850"/>
+            <a:gd name="connsiteX2" fmla="*/ 0 w 609600"/>
+            <a:gd name="connsiteY2" fmla="*/ 704850 h 704850"/>
+            <a:gd name="connsiteX0" fmla="*/ 590550 w 590550"/>
+            <a:gd name="connsiteY0" fmla="*/ 0 h 704850"/>
+            <a:gd name="connsiteX1" fmla="*/ 276225 w 590550"/>
+            <a:gd name="connsiteY1" fmla="*/ 171450 h 704850"/>
+            <a:gd name="connsiteX2" fmla="*/ 0 w 590550"/>
+            <a:gd name="connsiteY2" fmla="*/ 704850 h 704850"/>
+          </a:gdLst>
+          <a:ahLst/>
+          <a:cxnLst>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX0" y="connsiteY0"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX1" y="connsiteY1"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX2" y="connsiteY2"/>
+            </a:cxn>
+          </a:cxnLst>
+          <a:rect l="l" t="t" r="r" b="b"/>
+          <a:pathLst>
+            <a:path w="590550" h="704850">
+              <a:moveTo>
+                <a:pt x="590550" y="0"/>
+              </a:moveTo>
+              <a:cubicBezTo>
+                <a:pt x="411956" y="55562"/>
+                <a:pt x="374650" y="53975"/>
+                <a:pt x="276225" y="171450"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="177800" y="288925"/>
+                <a:pt x="59531" y="525462"/>
+                <a:pt x="0" y="704850"/>
+              </a:cubicBezTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="39" name="四角形: 角を丸くする 38">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{409F24F6-1600-473B-ACCF-6F33EE4F2B76}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2381250" y="1428750"/>
+          <a:ext cx="485775" cy="238126"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="40" name="四角形: 角を丸くする 39">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C99B1D8-D234-457D-AA52-D5A74876BF20}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5000625" y="1428750"/>
+          <a:ext cx="485775" cy="238126"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="42" name="四角形: 角を丸くする 41">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C7C7121-E3E4-497B-A647-52E9CD18BFFA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3571875" y="2381250"/>
+          <a:ext cx="723900" cy="238126"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>228600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>9526</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>228601</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="43" name="四角形: 角を丸くする 42">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2D490F12-4283-4B06-A5CB-3CA61CEE3D4B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3095626" y="2371725"/>
+          <a:ext cx="247650" cy="238126"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>9526</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>9526</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="44" name="四角形: 角を丸くする 43">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4AF91008-9D3E-4C7D-9C24-51B7875EFABB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4524376" y="2390775"/>
+          <a:ext cx="247650" cy="238126"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>9526</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="46" name="四角形: 角を丸くする 45">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8158281A-5F9F-4AA0-B18C-23F0237A5AEA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5238751" y="2143125"/>
+          <a:ext cx="247650" cy="238126"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>9526</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>28576</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="47" name="グラフィックス 46">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{291E5D34-0E05-1064-6D59-12D7C5BF26A1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5248276" y="2628900"/>
+          <a:ext cx="257175" cy="247650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>9526</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>19051</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>9526</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="48" name="四角形: 角を丸くする 47">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{085AD319-45EA-4843-A48E-FE71D31CDB8E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5010151" y="2390775"/>
+          <a:ext cx="247650" cy="238126"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>9526</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="49" name="四角形: 角を丸くする 48">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6D61F92E-0EF8-4FCD-A4DD-6581AD790425}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3095626" y="3095625"/>
+          <a:ext cx="247650" cy="238126"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>9526</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="54" name="四角形: 角を丸くする 53">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A1ECF432-FAE7-4544-9FFC-0298C6B6EA0F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5476876" y="2381250"/>
+          <a:ext cx="247650" cy="238126"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>9526</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>9526</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="55" name="四角形: 角を丸くする 54">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EB277F3A-A76F-442C-8DE6-47990036BEA2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3333751" y="3343275"/>
+          <a:ext cx="247650" cy="238126"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>9526</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>19051</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="56" name="四角形: 角を丸くする 55">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A2056A70-F4A2-410F-BDA0-4F3DE74EA992}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3105151" y="3571875"/>
+          <a:ext cx="247650" cy="238126"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>9526</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>19051</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="57" name="四角形: 角を丸くする 56">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2F676C5E-B0C5-4F62-BEC6-8B4B675B76E0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2867026" y="3333750"/>
+          <a:ext cx="247650" cy="238126"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1135,7 +2699,7 @@
       <c r="T4" s="2"/>
       <c r="U4" s="2"/>
       <c r="V4" s="3"/>
-      <c r="W4" s="4"/>
+      <c r="W4" s="3"/>
       <c r="X4" s="2"/>
       <c r="Y4" s="2"/>
       <c r="Z4" s="2"/>
@@ -1147,7 +2711,7 @@
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
-      <c r="L5" s="5">
+      <c r="L5" s="3">
         <v>6</v>
       </c>
       <c r="M5" s="2"/>
@@ -1159,10 +2723,10 @@
       <c r="S5" s="2"/>
       <c r="T5" s="2"/>
       <c r="U5" s="2"/>
-      <c r="V5" s="5">
+      <c r="V5" s="3">
         <v>7</v>
       </c>
-      <c r="W5" s="4"/>
+      <c r="W5" s="3"/>
       <c r="X5" s="2"/>
       <c r="Y5" s="2"/>
       <c r="Z5" s="2"/>
@@ -1196,8 +2760,8 @@
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="7">
+      <c r="K7" s="3"/>
+      <c r="L7" s="3">
         <v>4</v>
       </c>
       <c r="M7" s="2"/>
@@ -1209,10 +2773,10 @@
       <c r="S7" s="2"/>
       <c r="T7" s="2"/>
       <c r="U7" s="2"/>
-      <c r="V7" s="6">
+      <c r="V7" s="3">
         <v>5</v>
       </c>
-      <c r="W7" s="7"/>
+      <c r="W7" s="3"/>
       <c r="X7" s="2"/>
       <c r="Y7" s="2"/>
       <c r="Z7" s="2"/>
@@ -1268,9 +2832,9 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="8"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
       <c r="O10" s="2"/>
@@ -1280,11 +2844,11 @@
       <c r="S10" s="2"/>
       <c r="T10" s="2"/>
       <c r="U10" s="2"/>
-      <c r="V10" s="8"/>
-      <c r="W10" s="9">
+      <c r="V10" s="3"/>
+      <c r="W10" s="3">
         <v>3</v>
       </c>
-      <c r="X10" s="8"/>
+      <c r="X10" s="3"/>
       <c r="Y10" s="2"/>
       <c r="Z10" s="2"/>
       <c r="AA10" s="2"/>
@@ -1293,31 +2857,31 @@
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8">
+      <c r="J11" s="3"/>
+      <c r="K11" s="3">
         <v>10</v>
       </c>
-      <c r="L11" s="8"/>
+      <c r="L11" s="3"/>
       <c r="M11" s="2"/>
-      <c r="N11" s="9">
+      <c r="N11" s="3">
         <v>8</v>
       </c>
       <c r="O11" s="2"/>
-      <c r="P11" s="6"/>
-      <c r="Q11" s="10">
+      <c r="P11" s="3"/>
+      <c r="Q11" s="3">
         <v>16</v>
       </c>
-      <c r="R11" s="7"/>
+      <c r="R11" s="3"/>
       <c r="S11" s="2"/>
-      <c r="T11" s="9">
+      <c r="T11" s="3">
         <v>9</v>
       </c>
       <c r="U11" s="2"/>
-      <c r="V11" s="9">
+      <c r="V11" s="3">
         <v>2</v>
       </c>
-      <c r="W11" s="8"/>
-      <c r="X11" s="9">
+      <c r="W11" s="3"/>
+      <c r="X11" s="3">
         <v>1</v>
       </c>
       <c r="Y11" s="2"/>
@@ -1328,9 +2892,9 @@
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="8"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
       <c r="O12" s="2"/>
@@ -1340,11 +2904,11 @@
       <c r="S12" s="2"/>
       <c r="T12" s="2"/>
       <c r="U12" s="2"/>
-      <c r="V12" s="8"/>
-      <c r="W12" s="9">
+      <c r="V12" s="3"/>
+      <c r="W12" s="3">
         <v>0</v>
       </c>
-      <c r="X12" s="8"/>
+      <c r="X12" s="3"/>
       <c r="Y12" s="2"/>
       <c r="Z12" s="2"/>
       <c r="AA12" s="2"/>
@@ -1379,17 +2943,17 @@
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
-      <c r="M14" s="8"/>
-      <c r="N14" s="9">
+      <c r="M14" s="3"/>
+      <c r="N14" s="3">
         <v>12</v>
       </c>
-      <c r="O14" s="8"/>
+      <c r="O14" s="3"/>
       <c r="P14" s="2"/>
       <c r="Q14" s="2"/>
       <c r="R14" s="2"/>
-      <c r="S14" s="8"/>
-      <c r="T14" s="8"/>
-      <c r="U14" s="8"/>
+      <c r="S14" s="3"/>
+      <c r="T14" s="3"/>
+      <c r="U14" s="3"/>
       <c r="V14" s="2"/>
       <c r="W14" s="2"/>
       <c r="X14" s="2"/>
@@ -1404,21 +2968,21 @@
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
-      <c r="M15" s="9">
+      <c r="M15" s="3">
         <v>14</v>
       </c>
-      <c r="N15" s="8"/>
-      <c r="O15" s="9">
+      <c r="N15" s="3"/>
+      <c r="O15" s="3">
         <v>15</v>
       </c>
       <c r="P15" s="2"/>
       <c r="Q15" s="2"/>
       <c r="R15" s="2"/>
-      <c r="S15" s="8"/>
-      <c r="T15" s="8">
+      <c r="S15" s="3"/>
+      <c r="T15" s="3">
         <v>11</v>
       </c>
-      <c r="U15" s="8"/>
+      <c r="U15" s="3"/>
       <c r="V15" s="2"/>
       <c r="W15" s="2"/>
       <c r="X15" s="2"/>
@@ -1433,17 +2997,17 @@
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
-      <c r="M16" s="8"/>
-      <c r="N16" s="9">
+      <c r="M16" s="3"/>
+      <c r="N16" s="3">
         <v>13</v>
       </c>
-      <c r="O16" s="8"/>
+      <c r="O16" s="3"/>
       <c r="P16" s="2"/>
       <c r="Q16" s="2"/>
       <c r="R16" s="2"/>
-      <c r="S16" s="8"/>
-      <c r="T16" s="8"/>
-      <c r="U16" s="8"/>
+      <c r="S16" s="3"/>
+      <c r="T16" s="3"/>
+      <c r="U16" s="3"/>
       <c r="V16" s="2"/>
       <c r="W16" s="2"/>
       <c r="X16" s="2"/>
@@ -1504,17 +3068,17 @@
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
-      <c r="M19" s="11" t="s">
+      <c r="M19" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="N19" s="11"/>
-      <c r="O19" s="11"/>
-      <c r="P19" s="11"/>
-      <c r="Q19" s="11"/>
-      <c r="R19" s="11"/>
-      <c r="S19" s="11"/>
-      <c r="T19" s="11"/>
-      <c r="U19" s="11"/>
+      <c r="N19" s="4"/>
+      <c r="O19" s="4"/>
+      <c r="P19" s="4"/>
+      <c r="Q19" s="4"/>
+      <c r="R19" s="4"/>
+      <c r="S19" s="4"/>
+      <c r="T19" s="4"/>
+      <c r="U19" s="4"/>
       <c r="V19" s="2"/>
       <c r="W19" s="2"/>
       <c r="X19" s="2"/>

</xml_diff>

<commit_message>
Modified a gamepad diagram again
</commit_message>
<xml_diff>
--- a/HTML5-XInput-locations.xlsx
+++ b/HTML5-XInput-locations.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TAKIZAWA Yozo\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TAKIZAWA Yozo\github\ytaki0801.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F04D6430-5C8C-412F-9FFB-B9123DCCCE4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3B9AC39-A707-4897-8C80-DFB56543F99A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{38F73DDA-D621-463A-9F7D-10B89270610F}"/>
   </bookViews>
@@ -1664,72 +1664,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="42" name="四角形: 角を丸くする 41">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C7C7121-E3E4-497B-A647-52E9CD18BFFA}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3571875" y="2381250"/>
-          <a:ext cx="723900" cy="238126"/>
-        </a:xfrm>
-        <a:prstGeom prst="roundRect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:solidFill>
-            <a:sysClr val="windowText" lastClr="000000"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>1</xdr:colOff>
       <xdr:row>9</xdr:row>
@@ -2336,6 +2270,72 @@
           <a:ext cx="247650" cy="238126"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>133351</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>95251</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="楕円 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F2B4023-CB36-4786-BCFD-42FCCA557D4E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3705225" y="2276476"/>
+          <a:ext cx="438150" cy="438150"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
           <a:avLst/>
         </a:prstGeom>
         <a:noFill/>

</xml_diff>